<commit_message>
Added area column to identify printers
</commit_message>
<xml_diff>
--- a/printers_Inventory.xlsx
+++ b/printers_Inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setchyberre\code\Lexmark_ink_reviewer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setchyberre\code\test\Lexmark_ink_reviewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51F357B-E4F8-4A98-9D85-4D00CCA30304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D928B36C-18E6-4225-A56A-DA2DAC331323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{8E19709F-7210-45CD-8730-C9473516A42A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8E19709F-7210-45CD-8730-C9473516A42A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
   <si>
     <t>CX522ade</t>
   </si>
@@ -84,9 +84,6 @@
     <t>172.16.1.169</t>
   </si>
   <si>
-    <t>Créditos y cobranzas</t>
-  </si>
-  <si>
     <t>701925110DFD5R</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>172.16.1.225</t>
   </si>
   <si>
-    <t>Gestión Humana</t>
-  </si>
-  <si>
     <t>701821740G03W</t>
   </si>
   <si>
@@ -229,6 +223,27 @@
   </si>
   <si>
     <t>San Juan de Yapacany</t>
+  </si>
+  <si>
+    <t>Cred. Cob.</t>
+  </si>
+  <si>
+    <t>Siglas</t>
+  </si>
+  <si>
+    <t>Significado</t>
+  </si>
+  <si>
+    <t>Creditos y Cobranzas</t>
+  </si>
+  <si>
+    <t>G.H.</t>
+  </si>
+  <si>
+    <t>Gestion Humana</t>
+  </si>
+  <si>
+    <t>S.J. Yapacany</t>
   </si>
 </sst>
 </file>
@@ -624,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E35585D-B5D6-40D0-A1CE-91E09DDA65DC}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,21 +652,27 @@
     <col min="4" max="4" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,8 +685,14 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -678,8 +705,14 @@
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -692,8 +725,14 @@
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -707,7 +746,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -718,10 +757,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -732,147 +771,147 @@
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -880,13 +919,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -894,13 +933,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -908,13 +947,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -922,13 +961,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added email_sender which uses .env file to retrieve credentials, the mail takes a file and send it to the recipients
</commit_message>
<xml_diff>
--- a/printers_Inventory.xlsx
+++ b/printers_Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setchyberre\code\test\Lexmark_ink_reviewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D928B36C-18E6-4225-A56A-DA2DAC331323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF9FA4F-B0E5-48CA-8D50-25FE1852C3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8E19709F-7210-45CD-8730-C9473516A42A}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7785" xr2:uid="{8E19709F-7210-45CD-8730-C9473516A42A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>Pirai</t>
   </si>
   <si>
-    <t>San Juan de Yapacany</t>
-  </si>
-  <si>
     <t>Cred. Cob.</t>
   </si>
   <si>
@@ -243,7 +240,10 @@
     <t>Gestion Humana</t>
   </si>
   <si>
-    <t>S.J. Yapacany</t>
+    <t>S.J. Yapacani</t>
+  </si>
+  <si>
+    <t>San Juan de Yapacani</t>
   </si>
 </sst>
 </file>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E35585D-B5D6-40D0-A1CE-91E09DDA65DC}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,10 +666,10 @@
         <v>56</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -686,10 +686,10 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -706,10 +706,10 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -726,10 +726,10 @@
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -771,7 +771,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -967,7 +967,7 @@
         <v>52</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>